<commit_message>
finalizado proceso estadistico mayo
</commit_message>
<xml_diff>
--- a/116103D05.xlsx
+++ b/116103D05.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\FORMULARIOS 2025\MAYO 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pie diabético\Desktop\Main\ESTADISTICAS\SERIES_A\2025\05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF3B5ED-3BBE-4C91-AE4B-9D009CED970D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213D25C6-2C0B-45AB-87AF-183FE337E9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="o5cW5b4paWuCVnQmbt44d6XbQtGtLl694Xv4WIdF3JEm7W4aJkFoYYotGa2PciX3uS2LJIcvToR8bDzfTvCrjQ==" workbookSaltValue="32v++s8p+WdbSyV9sF4Yvw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="599" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOMBRE" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NOMBRE!$AA$12:$AC$42</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3635,12 +3646,213 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="70" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="62" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="70" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="70" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="62" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="19" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="71" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="91" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="101" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="103" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="105" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="99" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="100" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="102" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="104" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="92" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="93" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="94" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3650,14 +3862,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="57" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3665,42 +3883,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="60" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="75" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="76" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="19" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="71" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3719,18 +3934,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3746,216 +3949,57 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="70" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="70" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="70" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="62" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="75" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="76" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="62" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="19" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="71" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="70" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="91" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="57" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="92" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="93" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="94" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="101" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="103" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="105" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="99" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="100" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="102" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="104" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="9" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="68" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3963,39 +4007,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="19" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="71" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="70" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="70" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4496,8 +4507,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AH49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4543,15 +4554,25 @@
       <c r="B2" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2</v>
+      </c>
       <c r="H2" s="74"/>
       <c r="I2" s="75" t="str">
         <f>IF(OR(NOMBRE!C2="",NOMBRE!E2="",NOMBRE!D2="",NOMBRE!E2="",NOMBRE!F2="",NOMBRE!G2=""),"Falta Cód. Com.","")</f>
-        <v>Falta Cód. Com.</v>
+        <v/>
       </c>
       <c r="J2" s="77"/>
       <c r="K2" s="77"/>
@@ -4573,7 +4594,7 @@
       <c r="AD2" s="6"/>
       <c r="AG2" s="7">
         <f>IF(I2&gt;"",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4584,22 +4605,22 @@
         <v>169</v>
       </c>
       <c r="C3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F3" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
       </c>
       <c r="H3" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" s="76" t="str">
         <f>IF(OR(NOMBRE!C3="",NOMBRE!D3="",NOMBRE!E3="",NOMBRE!F3="",NOMBRE!G3="",NOMBRE!H3=""),"Falta Cód. Estab.","")</f>
@@ -4691,13 +4712,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="368" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6" s="369">
         <v>0</v>
       </c>
       <c r="D6" s="370">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -4739,7 +4760,7 @@
       </c>
       <c r="AG7" s="13">
         <f>SUM(AG2:AG6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -5527,7 +5548,7 @@
     <row r="2" spans="1:54" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="str">
         <f>CONCATENATE("COMUNA: ",NOMBRE!$B$2,"  ","( ",NOMBRE!$C$2,NOMBRE!$D$2,NOMBRE!$E$2,NOMBRE!$F$2,NOMBRE!$G$2," )")</f>
-        <v>COMUNA: HUALAÑÉ  (  )</v>
+        <v>COMUNA: HUALAÑÉ  ( 07302 )</v>
       </c>
       <c r="Z2" s="170"/>
       <c r="AA2" s="170"/>
@@ -5560,7 +5581,7 @@
     <row r="3" spans="1:54" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="str">
         <f>CONCATENATE("ESTABLECIMIENTO/ESTRATEGIA: ",NOMBRE!$B$3,"  ","( ",NOMBRE!$C$3,NOMBRE!$D$3,NOMBRE!$E$3,NOMBRE!$F$3,NOMBRE!$G$3,NOMBRE!$H$3," )")</f>
-        <v>ESTABLECIMIENTO/ESTRATEGIA: HOSPITAL DE HUALAÑÉ  ( 200501 )</v>
+        <v>ESTABLECIMIENTO/ESTRATEGIA: HOSPITAL DE HUALAÑÉ  ( 116103 )</v>
       </c>
       <c r="D3" s="25"/>
       <c r="Z3" s="170"/>
@@ -5594,7 +5615,7 @@
     <row r="4" spans="1:54" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="str">
         <f>CONCATENATE("MES: ",NOMBRE!$B$6,"  ","( ",NOMBRE!$C$6,NOMBRE!$D$6," )")</f>
-        <v>MES: ABRIL  ( 04 )</v>
+        <v>MES: MAYO  ( 05 )</v>
       </c>
       <c r="Z4" s="170"/>
       <c r="AA4" s="170"/>
@@ -5657,17 +5678,17 @@
       <c r="AZ5" s="170"/>
     </row>
     <row r="6" spans="1:54" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="674"/>
-      <c r="B6" s="674"/>
-      <c r="C6" s="674"/>
-      <c r="D6" s="674"/>
-      <c r="E6" s="674"/>
-      <c r="F6" s="674"/>
-      <c r="G6" s="674"/>
-      <c r="H6" s="674"/>
-      <c r="I6" s="674"/>
-      <c r="J6" s="674"/>
-      <c r="K6" s="674"/>
+      <c r="A6" s="637"/>
+      <c r="B6" s="637"/>
+      <c r="C6" s="637"/>
+      <c r="D6" s="637"/>
+      <c r="E6" s="637"/>
+      <c r="F6" s="637"/>
+      <c r="G6" s="637"/>
+      <c r="H6" s="637"/>
+      <c r="I6" s="637"/>
+      <c r="J6" s="637"/>
+      <c r="K6" s="637"/>
       <c r="L6" s="26"/>
       <c r="Z6" s="171"/>
       <c r="AA6" s="171"/>
@@ -5698,25 +5719,25 @@
       <c r="AZ6" s="171"/>
     </row>
     <row r="7" spans="1:54" s="27" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="675" t="s">
+      <c r="A7" s="638" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="675"/>
-      <c r="C7" s="675"/>
-      <c r="D7" s="675"/>
-      <c r="E7" s="675"/>
-      <c r="F7" s="675"/>
-      <c r="G7" s="675"/>
-      <c r="H7" s="675"/>
-      <c r="I7" s="675"/>
-      <c r="J7" s="675"/>
-      <c r="K7" s="675"/>
-      <c r="L7" s="675"/>
-      <c r="M7" s="675"/>
-      <c r="N7" s="675"/>
-      <c r="O7" s="675"/>
-      <c r="P7" s="675"/>
-      <c r="Q7" s="675"/>
+      <c r="B7" s="638"/>
+      <c r="C7" s="638"/>
+      <c r="D7" s="638"/>
+      <c r="E7" s="638"/>
+      <c r="F7" s="638"/>
+      <c r="G7" s="638"/>
+      <c r="H7" s="638"/>
+      <c r="I7" s="638"/>
+      <c r="J7" s="638"/>
+      <c r="K7" s="638"/>
+      <c r="L7" s="638"/>
+      <c r="M7" s="638"/>
+      <c r="N7" s="638"/>
+      <c r="O7" s="638"/>
+      <c r="P7" s="638"/>
+      <c r="Q7" s="638"/>
       <c r="Z7" s="171"/>
       <c r="AA7" s="171"/>
       <c r="AB7" s="171"/>
@@ -5752,117 +5773,117 @@
       <c r="B8" s="88"/>
     </row>
     <row r="9" spans="1:54" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="606" t="s">
+      <c r="A9" s="619" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="628" t="s">
+      <c r="B9" s="639" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="628" t="s">
+      <c r="C9" s="639" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="631" t="s">
+      <c r="D9" s="595" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="632"/>
-      <c r="F9" s="632"/>
-      <c r="G9" s="632"/>
-      <c r="H9" s="632"/>
-      <c r="I9" s="632"/>
-      <c r="J9" s="659"/>
-      <c r="K9" s="679" t="s">
+      <c r="E9" s="596"/>
+      <c r="F9" s="596"/>
+      <c r="G9" s="596"/>
+      <c r="H9" s="596"/>
+      <c r="I9" s="596"/>
+      <c r="J9" s="642"/>
+      <c r="K9" s="646" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="659"/>
-      <c r="M9" s="635" t="s">
+      <c r="L9" s="642"/>
+      <c r="M9" s="599" t="s">
         <v>66</v>
       </c>
-      <c r="N9" s="635"/>
-      <c r="O9" s="636"/>
+      <c r="N9" s="599"/>
+      <c r="O9" s="600"/>
       <c r="X9" s="167"/>
       <c r="Y9" s="167"/>
       <c r="AZ9" s="28"/>
     </row>
     <row r="10" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="607"/>
-      <c r="B10" s="629"/>
-      <c r="C10" s="629"/>
-      <c r="D10" s="637" t="s">
+      <c r="A10" s="620"/>
+      <c r="B10" s="640"/>
+      <c r="C10" s="640"/>
+      <c r="D10" s="587" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="640" t="s">
+      <c r="E10" s="590" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="643" t="s">
+      <c r="F10" s="601" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="646" t="s">
+      <c r="G10" s="604" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="643" t="s">
+      <c r="H10" s="601" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="643" t="s">
+      <c r="I10" s="601" t="s">
         <v>72</v>
       </c>
-      <c r="J10" s="662" t="s">
+      <c r="J10" s="650" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="680" t="s">
+      <c r="K10" s="647" t="s">
         <v>74</v>
       </c>
-      <c r="L10" s="676" t="s">
+      <c r="L10" s="643" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="615" t="s">
+      <c r="M10" s="616" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="589" t="s">
+      <c r="N10" s="656" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="656" t="s">
+      <c r="O10" s="653" t="s">
         <v>78</v>
       </c>
       <c r="Y10" s="167"/>
     </row>
     <row r="11" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="607"/>
-      <c r="B11" s="629"/>
-      <c r="C11" s="629"/>
-      <c r="D11" s="638"/>
-      <c r="E11" s="641"/>
-      <c r="F11" s="644"/>
-      <c r="G11" s="647"/>
-      <c r="H11" s="644"/>
-      <c r="I11" s="644"/>
-      <c r="J11" s="663"/>
-      <c r="K11" s="681"/>
-      <c r="L11" s="677"/>
-      <c r="M11" s="665"/>
-      <c r="N11" s="590"/>
-      <c r="O11" s="657"/>
+      <c r="A11" s="620"/>
+      <c r="B11" s="640"/>
+      <c r="C11" s="640"/>
+      <c r="D11" s="588"/>
+      <c r="E11" s="591"/>
+      <c r="F11" s="602"/>
+      <c r="G11" s="605"/>
+      <c r="H11" s="602"/>
+      <c r="I11" s="602"/>
+      <c r="J11" s="651"/>
+      <c r="K11" s="648"/>
+      <c r="L11" s="644"/>
+      <c r="M11" s="617"/>
+      <c r="N11" s="657"/>
+      <c r="O11" s="654"/>
       <c r="Y11" s="167"/>
     </row>
     <row r="12" spans="1:54" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="608"/>
-      <c r="B12" s="630"/>
-      <c r="C12" s="630"/>
-      <c r="D12" s="639"/>
-      <c r="E12" s="642"/>
-      <c r="F12" s="645"/>
-      <c r="G12" s="648"/>
-      <c r="H12" s="645"/>
-      <c r="I12" s="645"/>
-      <c r="J12" s="664"/>
-      <c r="K12" s="682"/>
-      <c r="L12" s="678"/>
-      <c r="M12" s="616"/>
-      <c r="N12" s="591"/>
-      <c r="O12" s="658"/>
+      <c r="A12" s="621"/>
+      <c r="B12" s="641"/>
+      <c r="C12" s="641"/>
+      <c r="D12" s="589"/>
+      <c r="E12" s="592"/>
+      <c r="F12" s="603"/>
+      <c r="G12" s="606"/>
+      <c r="H12" s="603"/>
+      <c r="I12" s="603"/>
+      <c r="J12" s="652"/>
+      <c r="K12" s="649"/>
+      <c r="L12" s="645"/>
+      <c r="M12" s="618"/>
+      <c r="N12" s="658"/>
+      <c r="O12" s="655"/>
       <c r="Y12" s="167"/>
     </row>
     <row r="13" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="607" t="s">
+      <c r="A13" s="620" t="s">
         <v>79</v>
       </c>
       <c r="B13" s="275" t="s">
@@ -5906,7 +5927,7 @@
       </c>
     </row>
     <row r="14" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="607"/>
+      <c r="A14" s="620"/>
       <c r="B14" s="275" t="s">
         <v>81</v>
       </c>
@@ -5954,7 +5975,7 @@
       <c r="AL14" s="554"/>
     </row>
     <row r="15" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="607"/>
+      <c r="A15" s="620"/>
       <c r="B15" s="275" t="s">
         <v>82</v>
       </c>
@@ -6008,7 +6029,7 @@
       <c r="BB15" s="167"/>
     </row>
     <row r="16" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="607"/>
+      <c r="A16" s="620"/>
       <c r="B16" s="275" t="s">
         <v>83</v>
       </c>
@@ -6045,7 +6066,7 @@
       </c>
     </row>
     <row r="17" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="608"/>
+      <c r="A17" s="621"/>
       <c r="B17" s="29" t="s">
         <v>84</v>
       </c>
@@ -6101,7 +6122,7 @@
       <c r="Y17" s="167"/>
     </row>
     <row r="18" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="607" t="s">
+      <c r="A18" s="620" t="s">
         <v>85</v>
       </c>
       <c r="B18" s="275" t="s">
@@ -6143,7 +6164,7 @@
       <c r="AH18" s="168"/>
     </row>
     <row r="19" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="607"/>
+      <c r="A19" s="620"/>
       <c r="B19" s="86" t="s">
         <v>81</v>
       </c>
@@ -6175,7 +6196,7 @@
       <c r="AH19" s="168"/>
     </row>
     <row r="20" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="607"/>
+      <c r="A20" s="620"/>
       <c r="B20" s="86" t="s">
         <v>86</v>
       </c>
@@ -6220,7 +6241,7 @@
       <c r="AH20" s="168"/>
     </row>
     <row r="21" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="607"/>
+      <c r="A21" s="620"/>
       <c r="B21" s="275" t="s">
         <v>82</v>
       </c>
@@ -6255,7 +6276,7 @@
       <c r="AF21" s="168"/>
     </row>
     <row r="22" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="607"/>
+      <c r="A22" s="620"/>
       <c r="B22" s="275" t="s">
         <v>83</v>
       </c>
@@ -6284,7 +6305,7 @@
       <c r="Y22" s="167"/>
     </row>
     <row r="23" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="608"/>
+      <c r="A23" s="621"/>
       <c r="B23" s="29" t="s">
         <v>84</v>
       </c>
@@ -6342,7 +6363,7 @@
       <c r="Y23" s="167"/>
     </row>
     <row r="24" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="606" t="s">
+      <c r="A24" s="619" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="86" t="s">
@@ -6382,7 +6403,7 @@
       <c r="AH24" s="168"/>
     </row>
     <row r="25" spans="1:52" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="607"/>
+      <c r="A25" s="620"/>
       <c r="B25" s="86" t="s">
         <v>89</v>
       </c>
@@ -6440,7 +6461,7 @@
       <c r="AZ25" s="169"/>
     </row>
     <row r="26" spans="1:52" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="607"/>
+      <c r="A26" s="620"/>
       <c r="B26" s="86" t="s">
         <v>86</v>
       </c>
@@ -6496,7 +6517,7 @@
       <c r="AZ26" s="169"/>
     </row>
     <row r="27" spans="1:52" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="608"/>
+      <c r="A27" s="621"/>
       <c r="B27" s="29" t="s">
         <v>84</v>
       </c>
@@ -6557,7 +6578,7 @@
       <c r="AZ27" s="169"/>
     </row>
     <row r="28" spans="1:52" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="606" t="s">
+      <c r="A28" s="619" t="s">
         <v>90</v>
       </c>
       <c r="B28" s="86" t="s">
@@ -6623,7 +6644,7 @@
       <c r="AZ28" s="169"/>
     </row>
     <row r="29" spans="1:52" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="607"/>
+      <c r="A29" s="620"/>
       <c r="B29" s="86" t="s">
         <v>92</v>
       </c>
@@ -6685,7 +6706,7 @@
       <c r="AZ29" s="169"/>
     </row>
     <row r="30" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="608"/>
+      <c r="A30" s="621"/>
       <c r="B30" s="29" t="s">
         <v>84</v>
       </c>
@@ -6731,10 +6752,10 @@
       <c r="Y30" s="167"/>
     </row>
     <row r="31" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="599" t="s">
+      <c r="A31" s="622" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="600"/>
+      <c r="B31" s="623"/>
       <c r="C31" s="408">
         <f>SUM(D31:O31)</f>
         <v>426.8</v>
@@ -6798,128 +6819,128 @@
       <c r="C32" s="32"/>
     </row>
     <row r="33" spans="1:54" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="603" t="s">
+      <c r="A33" s="624" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="592"/>
-      <c r="C33" s="606" t="s">
+      <c r="B33" s="625"/>
+      <c r="C33" s="619" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="606" t="s">
+      <c r="D33" s="619" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="606" t="s">
+      <c r="E33" s="619" t="s">
         <v>95</v>
       </c>
-      <c r="F33" s="631" t="s">
+      <c r="F33" s="595" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="632"/>
-      <c r="H33" s="632"/>
-      <c r="I33" s="632"/>
-      <c r="J33" s="632"/>
-      <c r="K33" s="632"/>
-      <c r="L33" s="659"/>
-      <c r="M33" s="660" t="s">
+      <c r="G33" s="596"/>
+      <c r="H33" s="596"/>
+      <c r="I33" s="596"/>
+      <c r="J33" s="596"/>
+      <c r="K33" s="596"/>
+      <c r="L33" s="642"/>
+      <c r="M33" s="659" t="s">
         <v>65</v>
       </c>
-      <c r="N33" s="661"/>
-      <c r="O33" s="634" t="s">
+      <c r="N33" s="660"/>
+      <c r="O33" s="598" t="s">
         <v>66</v>
       </c>
-      <c r="P33" s="635"/>
-      <c r="Q33" s="636"/>
+      <c r="P33" s="599"/>
+      <c r="Q33" s="600"/>
       <c r="S33" s="24"/>
     </row>
     <row r="34" spans="1:54" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="604"/>
-      <c r="B34" s="593"/>
-      <c r="C34" s="604"/>
-      <c r="D34" s="607"/>
-      <c r="E34" s="607"/>
-      <c r="F34" s="637" t="s">
+      <c r="A34" s="626"/>
+      <c r="B34" s="627"/>
+      <c r="C34" s="626"/>
+      <c r="D34" s="620"/>
+      <c r="E34" s="620"/>
+      <c r="F34" s="587" t="s">
         <v>67</v>
       </c>
-      <c r="G34" s="643" t="s">
+      <c r="G34" s="601" t="s">
         <v>68</v>
       </c>
-      <c r="H34" s="643" t="s">
+      <c r="H34" s="601" t="s">
         <v>69</v>
       </c>
-      <c r="I34" s="646" t="s">
+      <c r="I34" s="604" t="s">
         <v>70</v>
       </c>
-      <c r="J34" s="643" t="s">
+      <c r="J34" s="601" t="s">
         <v>71</v>
       </c>
-      <c r="K34" s="643" t="s">
+      <c r="K34" s="601" t="s">
         <v>72</v>
       </c>
-      <c r="L34" s="662" t="s">
+      <c r="L34" s="650" t="s">
         <v>73</v>
       </c>
-      <c r="M34" s="615" t="s">
+      <c r="M34" s="616" t="s">
         <v>74</v>
       </c>
-      <c r="N34" s="666" t="s">
+      <c r="N34" s="661" t="s">
         <v>75</v>
       </c>
-      <c r="O34" s="615" t="s">
+      <c r="O34" s="616" t="s">
         <v>76</v>
       </c>
-      <c r="P34" s="589" t="s">
+      <c r="P34" s="656" t="s">
         <v>77</v>
       </c>
-      <c r="Q34" s="592" t="s">
+      <c r="Q34" s="625" t="s">
         <v>78</v>
       </c>
       <c r="S34" s="24"/>
     </row>
     <row r="35" spans="1:54" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="604"/>
-      <c r="B35" s="593"/>
-      <c r="C35" s="604"/>
-      <c r="D35" s="607"/>
-      <c r="E35" s="607"/>
-      <c r="F35" s="638"/>
-      <c r="G35" s="644"/>
-      <c r="H35" s="644"/>
-      <c r="I35" s="647"/>
-      <c r="J35" s="644"/>
-      <c r="K35" s="644"/>
-      <c r="L35" s="663"/>
-      <c r="M35" s="665"/>
-      <c r="N35" s="667"/>
-      <c r="O35" s="665"/>
-      <c r="P35" s="590"/>
-      <c r="Q35" s="593"/>
+      <c r="A35" s="626"/>
+      <c r="B35" s="627"/>
+      <c r="C35" s="626"/>
+      <c r="D35" s="620"/>
+      <c r="E35" s="620"/>
+      <c r="F35" s="588"/>
+      <c r="G35" s="602"/>
+      <c r="H35" s="602"/>
+      <c r="I35" s="605"/>
+      <c r="J35" s="602"/>
+      <c r="K35" s="602"/>
+      <c r="L35" s="651"/>
+      <c r="M35" s="617"/>
+      <c r="N35" s="662"/>
+      <c r="O35" s="617"/>
+      <c r="P35" s="657"/>
+      <c r="Q35" s="627"/>
       <c r="S35" s="24"/>
     </row>
     <row r="36" spans="1:54" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="605"/>
-      <c r="B36" s="594"/>
-      <c r="C36" s="604"/>
-      <c r="D36" s="608"/>
-      <c r="E36" s="608"/>
-      <c r="F36" s="639"/>
-      <c r="G36" s="645"/>
-      <c r="H36" s="645"/>
-      <c r="I36" s="648"/>
-      <c r="J36" s="645"/>
-      <c r="K36" s="645"/>
-      <c r="L36" s="664"/>
-      <c r="M36" s="616"/>
-      <c r="N36" s="668"/>
-      <c r="O36" s="616"/>
-      <c r="P36" s="591"/>
-      <c r="Q36" s="594"/>
+      <c r="A36" s="628"/>
+      <c r="B36" s="629"/>
+      <c r="C36" s="626"/>
+      <c r="D36" s="621"/>
+      <c r="E36" s="621"/>
+      <c r="F36" s="589"/>
+      <c r="G36" s="603"/>
+      <c r="H36" s="603"/>
+      <c r="I36" s="606"/>
+      <c r="J36" s="603"/>
+      <c r="K36" s="603"/>
+      <c r="L36" s="652"/>
+      <c r="M36" s="618"/>
+      <c r="N36" s="663"/>
+      <c r="O36" s="618"/>
+      <c r="P36" s="658"/>
+      <c r="Q36" s="629"/>
       <c r="S36" s="24"/>
     </row>
     <row r="37" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="595" t="s">
+      <c r="A37" s="664" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="596"/>
+      <c r="B37" s="665"/>
       <c r="C37" s="172">
         <f>SUM(F37:Q37)</f>
         <v>181</v>
@@ -7067,10 +7088,10 @@
       <c r="BB38" s="167"/>
     </row>
     <row r="39" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="624" t="s">
+      <c r="A39" s="666" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="625"/>
+      <c r="B39" s="667"/>
       <c r="C39" s="125">
         <f>SUM(F39:H39)</f>
         <v>1</v>
@@ -7191,10 +7212,10 @@
       <c r="BB40" s="167"/>
     </row>
     <row r="41" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="626" t="s">
+      <c r="A41" s="668" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="627"/>
+      <c r="B41" s="669"/>
       <c r="C41" s="130">
         <f>SUM(D41:E41)</f>
         <v>195</v>
@@ -7271,10 +7292,10 @@
       <c r="BB41" s="167"/>
     </row>
     <row r="42" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="672" t="s">
+      <c r="A42" s="635" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="673"/>
+      <c r="B42" s="636"/>
       <c r="C42" s="130">
         <f>SUM(F42:Q42)</f>
         <v>0</v>
@@ -7350,114 +7371,114 @@
       <c r="AA45" s="168"/>
     </row>
     <row r="46" spans="1:54" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="606" t="s">
+      <c r="A46" s="619" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="628" t="s">
+      <c r="B46" s="639" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="628" t="s">
+      <c r="C46" s="639" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="631" t="s">
+      <c r="D46" s="595" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="632"/>
-      <c r="F46" s="632"/>
-      <c r="G46" s="632"/>
-      <c r="H46" s="632"/>
-      <c r="I46" s="632"/>
-      <c r="J46" s="632"/>
-      <c r="K46" s="631" t="s">
+      <c r="E46" s="596"/>
+      <c r="F46" s="596"/>
+      <c r="G46" s="596"/>
+      <c r="H46" s="596"/>
+      <c r="I46" s="596"/>
+      <c r="J46" s="596"/>
+      <c r="K46" s="595" t="s">
         <v>65</v>
       </c>
-      <c r="L46" s="633"/>
-      <c r="M46" s="634" t="s">
+      <c r="L46" s="597"/>
+      <c r="M46" s="598" t="s">
         <v>66</v>
       </c>
-      <c r="N46" s="635"/>
-      <c r="O46" s="636"/>
+      <c r="N46" s="599"/>
+      <c r="O46" s="600"/>
       <c r="AB46" s="168"/>
     </row>
     <row r="47" spans="1:54" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="607"/>
-      <c r="B47" s="629"/>
-      <c r="C47" s="629"/>
-      <c r="D47" s="637" t="s">
+      <c r="A47" s="620"/>
+      <c r="B47" s="640"/>
+      <c r="C47" s="640"/>
+      <c r="D47" s="587" t="s">
         <v>67</v>
       </c>
-      <c r="E47" s="640" t="s">
+      <c r="E47" s="590" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="643" t="s">
+      <c r="F47" s="601" t="s">
         <v>69</v>
       </c>
-      <c r="G47" s="646" t="s">
+      <c r="G47" s="604" t="s">
         <v>70</v>
       </c>
-      <c r="H47" s="643" t="s">
+      <c r="H47" s="601" t="s">
         <v>71</v>
       </c>
-      <c r="I47" s="643" t="s">
+      <c r="I47" s="601" t="s">
         <v>72</v>
       </c>
-      <c r="J47" s="649" t="s">
+      <c r="J47" s="670" t="s">
         <v>73</v>
       </c>
-      <c r="K47" s="652" t="s">
+      <c r="K47" s="610" t="s">
         <v>74</v>
       </c>
-      <c r="L47" s="617" t="s">
+      <c r="L47" s="613" t="s">
         <v>75</v>
       </c>
-      <c r="M47" s="652" t="s">
+      <c r="M47" s="610" t="s">
         <v>76</v>
       </c>
-      <c r="N47" s="589" t="s">
+      <c r="N47" s="656" t="s">
         <v>77</v>
       </c>
-      <c r="O47" s="656" t="s">
+      <c r="O47" s="653" t="s">
         <v>78</v>
       </c>
       <c r="AB47" s="168"/>
     </row>
     <row r="48" spans="1:54" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="607"/>
-      <c r="B48" s="629"/>
-      <c r="C48" s="629"/>
-      <c r="D48" s="638"/>
-      <c r="E48" s="641"/>
-      <c r="F48" s="644"/>
-      <c r="G48" s="647"/>
-      <c r="H48" s="644"/>
-      <c r="I48" s="644"/>
-      <c r="J48" s="650"/>
-      <c r="K48" s="653"/>
-      <c r="L48" s="655"/>
-      <c r="M48" s="653"/>
-      <c r="N48" s="590"/>
-      <c r="O48" s="657"/>
+      <c r="A48" s="620"/>
+      <c r="B48" s="640"/>
+      <c r="C48" s="640"/>
+      <c r="D48" s="588"/>
+      <c r="E48" s="591"/>
+      <c r="F48" s="602"/>
+      <c r="G48" s="605"/>
+      <c r="H48" s="602"/>
+      <c r="I48" s="602"/>
+      <c r="J48" s="671"/>
+      <c r="K48" s="611"/>
+      <c r="L48" s="614"/>
+      <c r="M48" s="611"/>
+      <c r="N48" s="657"/>
+      <c r="O48" s="654"/>
       <c r="AB48" s="168"/>
     </row>
     <row r="49" spans="1:37" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="608"/>
-      <c r="B49" s="630"/>
-      <c r="C49" s="630"/>
-      <c r="D49" s="639"/>
-      <c r="E49" s="642"/>
-      <c r="F49" s="645"/>
-      <c r="G49" s="648"/>
-      <c r="H49" s="645"/>
-      <c r="I49" s="645"/>
-      <c r="J49" s="651"/>
-      <c r="K49" s="654"/>
-      <c r="L49" s="618"/>
-      <c r="M49" s="654"/>
-      <c r="N49" s="591"/>
-      <c r="O49" s="658"/>
+      <c r="A49" s="621"/>
+      <c r="B49" s="641"/>
+      <c r="C49" s="641"/>
+      <c r="D49" s="589"/>
+      <c r="E49" s="592"/>
+      <c r="F49" s="603"/>
+      <c r="G49" s="606"/>
+      <c r="H49" s="603"/>
+      <c r="I49" s="603"/>
+      <c r="J49" s="672"/>
+      <c r="K49" s="612"/>
+      <c r="L49" s="615"/>
+      <c r="M49" s="612"/>
+      <c r="N49" s="658"/>
+      <c r="O49" s="655"/>
     </row>
     <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="607" t="s">
+      <c r="A50" s="620" t="s">
         <v>79</v>
       </c>
       <c r="B50" s="275" t="s">
@@ -7507,7 +7528,7 @@
       <c r="AI50" s="168"/>
     </row>
     <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="607"/>
+      <c r="A51" s="620"/>
       <c r="B51" s="275" t="s">
         <v>81</v>
       </c>
@@ -7543,7 +7564,7 @@
       <c r="AI51" s="168"/>
     </row>
     <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="607"/>
+      <c r="A52" s="620"/>
       <c r="B52" s="86" t="s">
         <v>82</v>
       </c>
@@ -7617,7 +7638,7 @@
       </c>
     </row>
     <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="607"/>
+      <c r="A53" s="620"/>
       <c r="B53" s="86" t="s">
         <v>83</v>
       </c>
@@ -7645,7 +7666,7 @@
       <c r="O53" s="137"/>
     </row>
     <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="608"/>
+      <c r="A54" s="621"/>
       <c r="B54" s="29" t="s">
         <v>84</v>
       </c>
@@ -7700,7 +7721,7 @@
       </c>
     </row>
     <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="607" t="s">
+      <c r="A55" s="620" t="s">
         <v>85</v>
       </c>
       <c r="B55" s="275" t="s">
@@ -7754,7 +7775,7 @@
       <c r="AI55" s="168"/>
     </row>
     <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="607"/>
+      <c r="A56" s="620"/>
       <c r="B56" s="86" t="s">
         <v>81</v>
       </c>
@@ -7792,7 +7813,7 @@
       <c r="AI56" s="168"/>
     </row>
     <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="607"/>
+      <c r="A57" s="620"/>
       <c r="B57" s="86" t="s">
         <v>86</v>
       </c>
@@ -7844,7 +7865,7 @@
       <c r="AI57" s="168"/>
     </row>
     <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="607"/>
+      <c r="A58" s="620"/>
       <c r="B58" s="86" t="s">
         <v>82</v>
       </c>
@@ -7878,7 +7899,7 @@
       <c r="AG58" s="168"/>
     </row>
     <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="607"/>
+      <c r="A59" s="620"/>
       <c r="B59" s="86" t="s">
         <v>83</v>
       </c>
@@ -7916,7 +7937,7 @@
       <c r="V59" s="278"/>
     </row>
     <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="608"/>
+      <c r="A60" s="621"/>
       <c r="B60" s="29" t="s">
         <v>84</v>
       </c>
@@ -7974,7 +7995,7 @@
       <c r="R60" s="30"/>
     </row>
     <row r="61" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="606" t="s">
+      <c r="A61" s="619" t="s">
         <v>87</v>
       </c>
       <c r="B61" s="86" t="s">
@@ -8014,7 +8035,7 @@
       <c r="AI61" s="168"/>
     </row>
     <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="607"/>
+      <c r="A62" s="620"/>
       <c r="B62" s="86" t="s">
         <v>89</v>
       </c>
@@ -8042,7 +8063,7 @@
       <c r="O62" s="116"/>
     </row>
     <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="607"/>
+      <c r="A63" s="620"/>
       <c r="B63" s="86" t="s">
         <v>86</v>
       </c>
@@ -8068,7 +8089,7 @@
       <c r="O63" s="227"/>
     </row>
     <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="608"/>
+      <c r="A64" s="621"/>
       <c r="B64" s="29" t="s">
         <v>84</v>
       </c>
@@ -8102,7 +8123,7 @@
       <c r="R64" s="30"/>
     </row>
     <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="603" t="s">
+      <c r="A65" s="624" t="s">
         <v>101</v>
       </c>
       <c r="B65" s="86" t="s">
@@ -8139,7 +8160,7 @@
       <c r="R65" s="30"/>
     </row>
     <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="604"/>
+      <c r="A66" s="626"/>
       <c r="B66" s="86" t="s">
         <v>92</v>
       </c>
@@ -8174,7 +8195,7 @@
       <c r="R66" s="30"/>
     </row>
     <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="605"/>
+      <c r="A67" s="628"/>
       <c r="B67" s="166" t="s">
         <v>84</v>
       </c>
@@ -8220,10 +8241,10 @@
       <c r="R67" s="30"/>
     </row>
     <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="599" t="s">
+      <c r="A68" s="622" t="s">
         <v>97</v>
       </c>
-      <c r="B68" s="600"/>
+      <c r="B68" s="623"/>
       <c r="C68" s="418">
         <f>SUM(D68:O68)</f>
         <v>0</v>
@@ -8307,128 +8328,128 @@
       <c r="C70" s="32"/>
     </row>
     <row r="71" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="603" t="s">
+      <c r="A71" s="624" t="s">
         <v>61</v>
       </c>
-      <c r="B71" s="592"/>
-      <c r="C71" s="606" t="s">
+      <c r="B71" s="625"/>
+      <c r="C71" s="619" t="s">
         <v>63</v>
       </c>
-      <c r="D71" s="606" t="s">
+      <c r="D71" s="619" t="s">
         <v>94</v>
       </c>
-      <c r="E71" s="606" t="s">
+      <c r="E71" s="619" t="s">
         <v>103</v>
       </c>
-      <c r="F71" s="631" t="s">
+      <c r="F71" s="595" t="s">
         <v>64</v>
       </c>
-      <c r="G71" s="632"/>
-      <c r="H71" s="632"/>
-      <c r="I71" s="632"/>
-      <c r="J71" s="632"/>
-      <c r="K71" s="632"/>
-      <c r="L71" s="633"/>
-      <c r="M71" s="631" t="s">
+      <c r="G71" s="596"/>
+      <c r="H71" s="596"/>
+      <c r="I71" s="596"/>
+      <c r="J71" s="596"/>
+      <c r="K71" s="596"/>
+      <c r="L71" s="597"/>
+      <c r="M71" s="595" t="s">
         <v>65</v>
       </c>
-      <c r="N71" s="633"/>
-      <c r="O71" s="634" t="s">
+      <c r="N71" s="597"/>
+      <c r="O71" s="598" t="s">
         <v>66</v>
       </c>
-      <c r="P71" s="635"/>
-      <c r="Q71" s="636"/>
+      <c r="P71" s="599"/>
+      <c r="Q71" s="600"/>
       <c r="S71" s="24"/>
     </row>
     <row r="72" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="604"/>
-      <c r="B72" s="593"/>
-      <c r="C72" s="604"/>
-      <c r="D72" s="607"/>
-      <c r="E72" s="607"/>
-      <c r="F72" s="637" t="s">
+      <c r="A72" s="626"/>
+      <c r="B72" s="627"/>
+      <c r="C72" s="626"/>
+      <c r="D72" s="620"/>
+      <c r="E72" s="620"/>
+      <c r="F72" s="587" t="s">
         <v>67</v>
       </c>
-      <c r="G72" s="640" t="s">
+      <c r="G72" s="590" t="s">
         <v>68</v>
       </c>
-      <c r="H72" s="643" t="s">
+      <c r="H72" s="601" t="s">
         <v>69</v>
       </c>
-      <c r="I72" s="646" t="s">
+      <c r="I72" s="604" t="s">
         <v>70</v>
       </c>
-      <c r="J72" s="643" t="s">
+      <c r="J72" s="601" t="s">
         <v>71</v>
       </c>
-      <c r="K72" s="643" t="s">
+      <c r="K72" s="601" t="s">
         <v>72</v>
       </c>
-      <c r="L72" s="685" t="s">
+      <c r="L72" s="607" t="s">
         <v>73</v>
       </c>
-      <c r="M72" s="652" t="s">
+      <c r="M72" s="610" t="s">
         <v>74</v>
       </c>
-      <c r="N72" s="617" t="s">
+      <c r="N72" s="613" t="s">
         <v>75</v>
       </c>
-      <c r="O72" s="615" t="s">
+      <c r="O72" s="616" t="s">
         <v>76</v>
       </c>
-      <c r="P72" s="589" t="s">
+      <c r="P72" s="656" t="s">
         <v>77</v>
       </c>
-      <c r="Q72" s="592" t="s">
+      <c r="Q72" s="625" t="s">
         <v>78</v>
       </c>
       <c r="S72" s="24"/>
     </row>
     <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="604"/>
-      <c r="B73" s="593"/>
-      <c r="C73" s="604"/>
-      <c r="D73" s="607"/>
-      <c r="E73" s="607"/>
-      <c r="F73" s="638"/>
-      <c r="G73" s="641"/>
-      <c r="H73" s="644"/>
-      <c r="I73" s="647"/>
-      <c r="J73" s="644"/>
-      <c r="K73" s="644"/>
-      <c r="L73" s="686"/>
-      <c r="M73" s="653"/>
-      <c r="N73" s="655"/>
-      <c r="O73" s="665"/>
-      <c r="P73" s="590"/>
-      <c r="Q73" s="593"/>
+      <c r="A73" s="626"/>
+      <c r="B73" s="627"/>
+      <c r="C73" s="626"/>
+      <c r="D73" s="620"/>
+      <c r="E73" s="620"/>
+      <c r="F73" s="588"/>
+      <c r="G73" s="591"/>
+      <c r="H73" s="602"/>
+      <c r="I73" s="605"/>
+      <c r="J73" s="602"/>
+      <c r="K73" s="602"/>
+      <c r="L73" s="608"/>
+      <c r="M73" s="611"/>
+      <c r="N73" s="614"/>
+      <c r="O73" s="617"/>
+      <c r="P73" s="657"/>
+      <c r="Q73" s="627"/>
       <c r="S73" s="24"/>
     </row>
     <row r="74" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="605"/>
-      <c r="B74" s="594"/>
-      <c r="C74" s="604"/>
-      <c r="D74" s="608"/>
-      <c r="E74" s="608"/>
-      <c r="F74" s="639"/>
-      <c r="G74" s="642"/>
-      <c r="H74" s="645"/>
-      <c r="I74" s="648"/>
-      <c r="J74" s="645"/>
-      <c r="K74" s="645"/>
-      <c r="L74" s="687"/>
-      <c r="M74" s="654"/>
-      <c r="N74" s="618"/>
-      <c r="O74" s="616"/>
-      <c r="P74" s="591"/>
-      <c r="Q74" s="594"/>
+      <c r="A74" s="628"/>
+      <c r="B74" s="629"/>
+      <c r="C74" s="626"/>
+      <c r="D74" s="621"/>
+      <c r="E74" s="621"/>
+      <c r="F74" s="589"/>
+      <c r="G74" s="592"/>
+      <c r="H74" s="603"/>
+      <c r="I74" s="606"/>
+      <c r="J74" s="603"/>
+      <c r="K74" s="603"/>
+      <c r="L74" s="609"/>
+      <c r="M74" s="612"/>
+      <c r="N74" s="615"/>
+      <c r="O74" s="618"/>
+      <c r="P74" s="658"/>
+      <c r="Q74" s="629"/>
       <c r="S74" s="24"/>
     </row>
     <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="595" t="s">
+      <c r="A75" s="664" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="596"/>
+      <c r="B75" s="665"/>
       <c r="C75" s="121">
         <f>SUM(F75:Q75)</f>
         <v>0</v>
@@ -8578,10 +8599,10 @@
       <c r="AM76" s="554"/>
     </row>
     <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="683" t="s">
+      <c r="A77" s="593" t="s">
         <v>87</v>
       </c>
-      <c r="B77" s="684"/>
+      <c r="B77" s="594"/>
       <c r="C77" s="160">
         <f>SUM(F77:H77)</f>
         <v>0</v>
@@ -8640,10 +8661,10 @@
       <c r="AM77" s="554"/>
     </row>
     <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="597" t="s">
+      <c r="A78" s="673" t="s">
         <v>104</v>
       </c>
-      <c r="B78" s="598"/>
+      <c r="B78" s="674"/>
       <c r="C78" s="150">
         <f>SUM(F78:L78)</f>
         <v>0</v>
@@ -8706,10 +8727,10 @@
       <c r="AM78" s="554"/>
     </row>
     <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="599" t="s">
+      <c r="A79" s="622" t="s">
         <v>97</v>
       </c>
-      <c r="B79" s="600"/>
+      <c r="B79" s="623"/>
       <c r="C79" s="150">
         <f>SUM(D79:E79)</f>
         <v>0</v>
@@ -8791,10 +8812,10 @@
       <c r="AM79" s="28"/>
     </row>
     <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="601" t="s">
+      <c r="A80" s="675" t="s">
         <v>98</v>
       </c>
-      <c r="B80" s="602"/>
+      <c r="B80" s="676"/>
       <c r="C80" s="130">
         <f>SUM(F80:Q80)</f>
         <v>0</v>
@@ -8919,30 +8940,30 @@
       <c r="AI83" s="168"/>
     </row>
     <row r="84" spans="1:439" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="603" t="s">
+      <c r="A84" s="624" t="s">
         <v>62</v>
       </c>
-      <c r="B84" s="592"/>
-      <c r="C84" s="606" t="s">
+      <c r="B84" s="625"/>
+      <c r="C84" s="619" t="s">
         <v>106</v>
       </c>
-      <c r="D84" s="609" t="s">
+      <c r="D84" s="677" t="s">
         <v>107</v>
       </c>
-      <c r="E84" s="610"/>
-      <c r="F84" s="606" t="s">
+      <c r="E84" s="678"/>
+      <c r="F84" s="619" t="s">
         <v>108</v>
       </c>
-      <c r="G84" s="613" t="s">
+      <c r="G84" s="681" t="s">
         <v>109</v>
       </c>
-      <c r="H84" s="613"/>
-      <c r="I84" s="613"/>
-      <c r="J84" s="613"/>
-      <c r="K84" s="613"/>
-      <c r="L84" s="613"/>
-      <c r="M84" s="613"/>
-      <c r="N84" s="614" t="s">
+      <c r="H84" s="681"/>
+      <c r="I84" s="681"/>
+      <c r="J84" s="681"/>
+      <c r="K84" s="681"/>
+      <c r="L84" s="681"/>
+      <c r="M84" s="681"/>
+      <c r="N84" s="682" t="s">
         <v>110</v>
       </c>
       <c r="P84" s="24"/>
@@ -8958,34 +8979,34 @@
       <c r="AG84" s="168"/>
     </row>
     <row r="85" spans="1:439" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="604"/>
-      <c r="B85" s="593"/>
-      <c r="C85" s="607"/>
-      <c r="D85" s="615" t="s">
+      <c r="A85" s="626"/>
+      <c r="B85" s="627"/>
+      <c r="C85" s="620"/>
+      <c r="D85" s="616" t="s">
         <v>111</v>
       </c>
-      <c r="E85" s="617" t="s">
+      <c r="E85" s="613" t="s">
         <v>112</v>
       </c>
-      <c r="F85" s="611"/>
-      <c r="G85" s="619" t="s">
+      <c r="F85" s="679"/>
+      <c r="G85" s="683" t="s">
         <v>113</v>
       </c>
-      <c r="H85" s="619"/>
-      <c r="I85" s="619"/>
-      <c r="J85" s="620" t="s">
+      <c r="H85" s="683"/>
+      <c r="I85" s="683"/>
+      <c r="J85" s="684" t="s">
         <v>114</v>
       </c>
-      <c r="K85" s="621" t="s">
+      <c r="K85" s="685" t="s">
         <v>115</v>
       </c>
-      <c r="L85" s="622" t="s">
+      <c r="L85" s="686" t="s">
         <v>116</v>
       </c>
-      <c r="M85" s="623" t="s">
+      <c r="M85" s="687" t="s">
         <v>117</v>
       </c>
-      <c r="N85" s="611"/>
+      <c r="N85" s="679"/>
       <c r="P85" s="24"/>
       <c r="X85" s="167"/>
       <c r="Y85" s="168"/>
@@ -8999,12 +9020,12 @@
       <c r="AG85" s="168"/>
     </row>
     <row r="86" spans="1:439" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="605"/>
-      <c r="B86" s="594"/>
-      <c r="C86" s="608"/>
-      <c r="D86" s="616"/>
-      <c r="E86" s="618"/>
-      <c r="F86" s="612"/>
+      <c r="A86" s="628"/>
+      <c r="B86" s="629"/>
+      <c r="C86" s="621"/>
+      <c r="D86" s="618"/>
+      <c r="E86" s="615"/>
+      <c r="F86" s="680"/>
       <c r="G86" s="33" t="s">
         <v>118</v>
       </c>
@@ -9014,11 +9035,11 @@
       <c r="I86" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="J86" s="620"/>
-      <c r="K86" s="591"/>
-      <c r="L86" s="622"/>
-      <c r="M86" s="623"/>
-      <c r="N86" s="612"/>
+      <c r="J86" s="684"/>
+      <c r="K86" s="658"/>
+      <c r="L86" s="686"/>
+      <c r="M86" s="687"/>
+      <c r="N86" s="680"/>
       <c r="P86" s="24"/>
       <c r="X86" s="167"/>
       <c r="Y86" s="168"/>
@@ -9150,10 +9171,10 @@
       <c r="AG88" s="168"/>
     </row>
     <row r="89" spans="1:439" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="587" t="s">
+      <c r="A89" s="630" t="s">
         <v>86</v>
       </c>
-      <c r="B89" s="588"/>
+      <c r="B89" s="631"/>
       <c r="C89" s="404">
         <v>48</v>
       </c>
@@ -9209,10 +9230,10 @@
       <c r="AG89" s="168"/>
     </row>
     <row r="90" spans="1:439" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="587" t="s">
+      <c r="A90" s="630" t="s">
         <v>82</v>
       </c>
-      <c r="B90" s="588"/>
+      <c r="B90" s="631"/>
       <c r="C90" s="405">
         <v>40</v>
       </c>
@@ -9268,10 +9289,10 @@
       <c r="AG90" s="168"/>
     </row>
     <row r="91" spans="1:439" s="179" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="587" t="s">
+      <c r="A91" s="630" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="588"/>
+      <c r="B91" s="631"/>
       <c r="C91" s="465">
         <v>122.4</v>
       </c>
@@ -9739,10 +9760,10 @@
       <c r="PW91" s="24"/>
     </row>
     <row r="92" spans="1:439" s="179" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="587" t="s">
+      <c r="A92" s="630" t="s">
         <v>120</v>
       </c>
-      <c r="B92" s="588"/>
+      <c r="B92" s="631"/>
       <c r="C92" s="470">
         <v>2.4</v>
       </c>
@@ -10212,10 +10233,10 @@
       <c r="PW92" s="24"/>
     </row>
     <row r="93" spans="1:439" s="179" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="587" t="s">
+      <c r="A93" s="630" t="s">
         <v>91</v>
       </c>
-      <c r="B93" s="588"/>
+      <c r="B93" s="631"/>
       <c r="C93" s="476">
         <v>3.2</v>
       </c>
@@ -10685,10 +10706,10 @@
       <c r="PW93" s="24"/>
     </row>
     <row r="94" spans="1:439" s="179" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="669" t="s">
+      <c r="A94" s="632" t="s">
         <v>121</v>
       </c>
-      <c r="B94" s="670"/>
+      <c r="B94" s="633"/>
       <c r="C94" s="482">
         <v>0</v>
       </c>
@@ -11158,10 +11179,10 @@
       <c r="PW94" s="24"/>
     </row>
     <row r="95" spans="1:439" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="671" t="s">
+      <c r="A95" s="634" t="s">
         <v>122</v>
       </c>
-      <c r="B95" s="671"/>
+      <c r="B95" s="634"/>
       <c r="C95" s="444">
         <f t="shared" ref="C95:N95" si="25">SUM(C87,C88:C94)</f>
         <v>1093.0000000000002</v>
@@ -11253,6 +11274,97 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="+uX8G/7V6BB++2DcurGBCAce1X5Vp1CFx0gYcnmfr68ZLjjYl2eA+ganqd/W9hYO4fs62DbGtYOHnETnnuvVCQ==" saltValue="LZ23QGH8dnDLt44sb9SdFg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="115">
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="P72:P74"/>
+    <mergeCell ref="Q72:Q74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A84:B86"/>
+    <mergeCell ref="C84:C86"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="F84:F86"/>
+    <mergeCell ref="G84:M84"/>
+    <mergeCell ref="N84:N86"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="J85:J86"/>
+    <mergeCell ref="K85:K86"/>
+    <mergeCell ref="L85:L86"/>
+    <mergeCell ref="M85:M86"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A71:B74"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="I47:I49"/>
+    <mergeCell ref="J47:J49"/>
+    <mergeCell ref="K47:K49"/>
+    <mergeCell ref="L47:L49"/>
+    <mergeCell ref="M47:M49"/>
+    <mergeCell ref="N47:N49"/>
+    <mergeCell ref="O47:O49"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="M34:M36"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="O34:O36"/>
+    <mergeCell ref="P34:P36"/>
+    <mergeCell ref="Q34:Q36"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A7:Q7"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="M10:M12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="G10:G12"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="A77:B77"/>
@@ -11277,97 +11389,6 @@
     <mergeCell ref="A33:B36"/>
     <mergeCell ref="C33:C36"/>
     <mergeCell ref="D33:D36"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A7:Q7"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="M10:M12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="M34:M36"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="O34:O36"/>
-    <mergeCell ref="P34:P36"/>
-    <mergeCell ref="Q34:Q36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="G47:G49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="I47:I49"/>
-    <mergeCell ref="J47:J49"/>
-    <mergeCell ref="K47:K49"/>
-    <mergeCell ref="L47:L49"/>
-    <mergeCell ref="M47:M49"/>
-    <mergeCell ref="N47:N49"/>
-    <mergeCell ref="O47:O49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A71:B74"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="P72:P74"/>
-    <mergeCell ref="Q72:Q74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A84:B86"/>
-    <mergeCell ref="C84:C86"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="F84:F86"/>
-    <mergeCell ref="G84:M84"/>
-    <mergeCell ref="N84:N86"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="G85:I85"/>
-    <mergeCell ref="J85:J86"/>
-    <mergeCell ref="K85:K86"/>
-    <mergeCell ref="L85:L86"/>
-    <mergeCell ref="M85:M86"/>
-    <mergeCell ref="A89:B89"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <dataValidations count="24">
@@ -11456,7 +11477,7 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:AC210"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
@@ -11494,20 +11515,20 @@
     <row r="2" spans="1:29" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="str">
         <f>CONCATENATE("COMUNA: ",NOMBRE!$B$2,"  ","( ",NOMBRE!$C$2,NOMBRE!$D$2,NOMBRE!$E$2,NOMBRE!$F$2,NOMBRE!$G$2," )")</f>
-        <v>COMUNA: HUALAÑÉ  (  )</v>
+        <v>COMUNA: HUALAÑÉ  ( 07302 )</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="str">
         <f>CONCATENATE("ESTABLECIMIENTO/ESTRATEGIA: ",NOMBRE!$B$3,"  ","( ",NOMBRE!$C$3,NOMBRE!$D$3,NOMBRE!$E$3,NOMBRE!$F$3,NOMBRE!$G$3,NOMBRE!$H$3," )")</f>
-        <v>ESTABLECIMIENTO/ESTRATEGIA: HOSPITAL DE HUALAÑÉ  ( 200501 )</v>
+        <v>ESTABLECIMIENTO/ESTRATEGIA: HOSPITAL DE HUALAÑÉ  ( 116103 )</v>
       </c>
       <c r="D3" s="25"/>
     </row>
     <row r="4" spans="1:29" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="str">
         <f>CONCATENATE("MES: ",NOMBRE!$B$6,"  ","( ",NOMBRE!$C$6,NOMBRE!$D$6," )")</f>
-        <v>MES: ABRIL  ( 04 )</v>
+        <v>MES: MAYO  ( 05 )</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11530,15 +11551,15 @@
       <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:29" s="40" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="688" t="s">
+      <c r="A7" s="702" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="688"/>
-      <c r="C7" s="688"/>
-      <c r="D7" s="688"/>
-      <c r="E7" s="688"/>
-      <c r="F7" s="688"/>
-      <c r="G7" s="688"/>
+      <c r="B7" s="702"/>
+      <c r="C7" s="702"/>
+      <c r="D7" s="702"/>
+      <c r="E7" s="702"/>
+      <c r="F7" s="702"/>
+      <c r="G7" s="702"/>
       <c r="H7" s="41"/>
       <c r="I7" s="41"/>
       <c r="J7" s="41"/>
@@ -11568,11 +11589,11 @@
       <c r="P8" s="41"/>
     </row>
     <row r="9" spans="1:29" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="696" t="s">
+      <c r="A9" s="707" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="696"/>
-      <c r="C9" s="696"/>
+      <c r="B9" s="707"/>
+      <c r="C9" s="707"/>
     </row>
     <row r="10" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="100" t="s">
@@ -11719,12 +11740,12 @@
       <c r="C17" s="274"/>
     </row>
     <row r="18" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="696" t="s">
+      <c r="A18" s="707" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="696"/>
-      <c r="C18" s="696"/>
-      <c r="D18" s="696"/>
+      <c r="B18" s="707"/>
+      <c r="C18" s="707"/>
+      <c r="D18" s="707"/>
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
       <c r="G18" s="40"/>
@@ -11734,17 +11755,17 @@
       <c r="K18" s="40"/>
     </row>
     <row r="19" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="689" t="s">
+      <c r="A19" s="688" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="697" t="s">
+      <c r="B19" s="698" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="698"/>
-      <c r="D19" s="699"/>
+      <c r="C19" s="699"/>
+      <c r="D19" s="700"/>
     </row>
     <row r="20" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="693"/>
+      <c r="A20" s="689"/>
       <c r="B20" s="280" t="s">
         <v>63</v>
       </c>
@@ -11962,84 +11983,84 @@
       <c r="AC27" s="72"/>
     </row>
     <row r="28" spans="1:29" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="696" t="s">
+      <c r="A28" s="707" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="696"/>
-      <c r="C28" s="696"/>
-      <c r="D28" s="696"/>
-      <c r="E28" s="696"/>
-      <c r="F28" s="696"/>
-      <c r="G28" s="696"/>
-      <c r="H28" s="696"/>
-      <c r="I28" s="696"/>
-      <c r="J28" s="696"/>
-      <c r="K28" s="696"/>
+      <c r="B28" s="707"/>
+      <c r="C28" s="707"/>
+      <c r="D28" s="707"/>
+      <c r="E28" s="707"/>
+      <c r="F28" s="707"/>
+      <c r="G28" s="707"/>
+      <c r="H28" s="707"/>
+      <c r="I28" s="707"/>
+      <c r="J28" s="707"/>
+      <c r="K28" s="707"/>
     </row>
     <row r="29" spans="1:29" s="87" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="689" t="s">
+      <c r="A29" s="688" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="689" t="s">
+      <c r="B29" s="688" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="705" t="s">
+      <c r="C29" s="696" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="706"/>
-      <c r="E29" s="689" t="s">
+      <c r="D29" s="697"/>
+      <c r="E29" s="688" t="s">
         <v>140</v>
       </c>
-      <c r="F29" s="700" t="s">
+      <c r="F29" s="690" t="s">
         <v>109</v>
       </c>
-      <c r="G29" s="701"/>
-      <c r="H29" s="701"/>
-      <c r="I29" s="701"/>
-      <c r="J29" s="702"/>
-      <c r="K29" s="689" t="s">
+      <c r="G29" s="691"/>
+      <c r="H29" s="691"/>
+      <c r="I29" s="691"/>
+      <c r="J29" s="692"/>
+      <c r="K29" s="688" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:29" s="87" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="692"/>
-      <c r="B30" s="692"/>
-      <c r="C30" s="703" t="s">
+      <c r="A30" s="695"/>
+      <c r="B30" s="695"/>
+      <c r="C30" s="693" t="s">
         <v>111</v>
       </c>
-      <c r="D30" s="694" t="s">
+      <c r="D30" s="705" t="s">
         <v>112</v>
       </c>
-      <c r="E30" s="692"/>
-      <c r="F30" s="606" t="s">
+      <c r="E30" s="695"/>
+      <c r="F30" s="619" t="s">
         <v>141</v>
       </c>
-      <c r="G30" s="615" t="s">
+      <c r="G30" s="616" t="s">
         <v>114</v>
       </c>
-      <c r="H30" s="589" t="s">
+      <c r="H30" s="656" t="s">
         <v>142</v>
       </c>
-      <c r="I30" s="592" t="s">
+      <c r="I30" s="625" t="s">
         <v>116</v>
       </c>
-      <c r="J30" s="593" t="s">
+      <c r="J30" s="627" t="s">
         <v>143</v>
       </c>
-      <c r="K30" s="690"/>
+      <c r="K30" s="703"/>
     </row>
     <row r="31" spans="1:29" s="87" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="693"/>
-      <c r="B31" s="693"/>
-      <c r="C31" s="704"/>
-      <c r="D31" s="695"/>
-      <c r="E31" s="693"/>
-      <c r="F31" s="608"/>
-      <c r="G31" s="616"/>
-      <c r="H31" s="591"/>
-      <c r="I31" s="594"/>
-      <c r="J31" s="668"/>
-      <c r="K31" s="691"/>
+      <c r="A31" s="689"/>
+      <c r="B31" s="689"/>
+      <c r="C31" s="694"/>
+      <c r="D31" s="706"/>
+      <c r="E31" s="689"/>
+      <c r="F31" s="621"/>
+      <c r="G31" s="618"/>
+      <c r="H31" s="658"/>
+      <c r="I31" s="629"/>
+      <c r="J31" s="663"/>
+      <c r="K31" s="704"/>
     </row>
     <row r="32" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="284" t="s">
@@ -12139,14 +12160,14 @@
       <c r="U34" s="70"/>
     </row>
     <row r="35" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="707" t="s">
+      <c r="A35" s="701" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="707"/>
-      <c r="C35" s="707"/>
-      <c r="D35" s="707"/>
-      <c r="E35" s="707"/>
-      <c r="F35" s="707"/>
+      <c r="B35" s="701"/>
+      <c r="C35" s="701"/>
+      <c r="D35" s="701"/>
+      <c r="E35" s="701"/>
+      <c r="F35" s="701"/>
       <c r="I35" s="37"/>
       <c r="J35" s="37"/>
       <c r="K35" s="37"/>
@@ -12156,21 +12177,21 @@
       <c r="O35" s="37"/>
     </row>
     <row r="36" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="689" t="s">
+      <c r="A36" s="688" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="697" t="s">
+      <c r="B36" s="698" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="698"/>
-      <c r="D36" s="699"/>
+      <c r="C36" s="699"/>
+      <c r="D36" s="700"/>
       <c r="E36" s="37"/>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
       <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="693"/>
+      <c r="A37" s="689"/>
       <c r="B37" s="280" t="s">
         <v>63</v>
       </c>
@@ -12347,14 +12368,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="5q8QtyhzzA3FDN9Ht/GB7eYdTaSv86S59xPoOrbua1yf5jvnR6GMf5tUU4uHXitt0Oq/mJfmX66LAS2clDtrqw==" saltValue="kBODPST6nWMczIc3+vJvxg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="22">
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="A35:F35"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="K29:K31"/>
     <mergeCell ref="E29:E31"/>
@@ -12369,6 +12382,14 @@
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="A35:F35"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <dataValidations count="3">
@@ -12394,7 +12415,7 @@
   <dimension ref="A1:N120"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12465,7 +12486,7 @@
       <c r="B4" s="44"/>
       <c r="C4" s="78" t="str">
         <f>CONCATENATE("ESTABLECIMIENTO/ESTRATEGIA: ",NOMBRE!B3," - ","( ",NOMBRE!C3,NOMBRE!D3,NOMBRE!E3,NOMBRE!F3,NOMBRE!G3,NOMBRE!H3," )")</f>
-        <v>ESTABLECIMIENTO/ESTRATEGIA: HOSPITAL DE HUALAÑÉ - ( 200501 )</v>
+        <v>ESTABLECIMIENTO/ESTRATEGIA: HOSPITAL DE HUALAÑÉ - ( 116103 )</v>
       </c>
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
@@ -12507,7 +12528,7 @@
       </c>
       <c r="E6" s="61" t="str">
         <f>IF((NOMBRE!AG7)=0,"","SIN INFORMACIÓN")</f>
-        <v>SIN INFORMACIÓN</v>
+        <v/>
       </c>
       <c r="F6" s="62"/>
       <c r="G6" s="62"/>
@@ -12586,7 +12607,7 @@
       </c>
       <c r="E10" s="65">
         <f>COUNTIF(E6:E8,"SIN INFORMACIÓN")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="62"/>
       <c r="G10" s="62"/>
@@ -12645,7 +12666,7 @@
       </c>
       <c r="E13" s="65">
         <f>SUM(E10:E12)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="44"/>
       <c r="G13" s="44"/>
@@ -12718,7 +12739,7 @@
       <c r="D18" s="49"/>
       <c r="E18" s="67">
         <f>NOMBRE!AG7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="49"/>
       <c r="G18" s="49"/>
@@ -13081,7 +13102,7 @@
     <row r="100" spans="5:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="E100" s="71">
         <f>NOMBRE!AG7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13143,7 +13164,7 @@
     <row r="4" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="79" t="str">
         <f>CONCATENATE("ESTABLECIMIENTO/ESTRATEGIA: ",NOMBRE!B3," - ","( ",NOMBRE!C3,NOMBRE!D3,NOMBRE!E3,NOMBRE!F3,NOMBRE!G3,NOMBRE!H3,NOMBRE!I3," )")</f>
-        <v>ESTABLECIMIENTO/ESTRATEGIA: HOSPITAL DE HUALAÑÉ - ( 200501 )</v>
+        <v>ESTABLECIMIENTO/ESTRATEGIA: HOSPITAL DE HUALAÑÉ - ( 116103 )</v>
       </c>
       <c r="C4" s="258"/>
       <c r="D4" s="258"/>
@@ -13202,7 +13223,7 @@
     <row r="10" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="711" t="str">
         <f>IF(Control!E13&gt;0,"ANTES DE EJECUTAR SUS MACROS REVISE LA HOJA CONTROL, EXISTEN ERRORES QUE DEBE CORREGIR","")</f>
-        <v>ANTES DE EJECUTAR SUS MACROS REVISE LA HOJA CONTROL, EXISTEN ERRORES QUE DEBE CORREGIR</v>
+        <v/>
       </c>
       <c r="C10" s="712"/>
       <c r="D10" s="712"/>

</xml_diff>